<commit_message>
Eliminado el excel y un bug a medias
</commit_message>
<xml_diff>
--- a/WineCompany.xlsx
+++ b/WineCompany.xlsx
@@ -1,29 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herre\Desktop\Proyecto Modela\PModela\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aldair Estrada\Documents\2S 2020\Modelacion y Simulacion 1\Clase Laboratorio\Proyecto\PModela\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1714EFCF-A6D1-48C8-9897-553B56B98B52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862A6F5F-573A-44F2-B9CE-FA5974B967DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elaboracion_Vino" sheetId="1" r:id="rId1"/>
-    <sheet name="Resultados_ElaboracionVino" sheetId="4" r:id="rId2"/>
-    <sheet name="Distribucion_Ordenes" sheetId="2" r:id="rId3"/>
-    <sheet name="Ventas" sheetId="3" r:id="rId4"/>
+    <sheet name="Distribucion_Ordenes" sheetId="2" r:id="rId2"/>
+    <sheet name="Ventas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -240,13 +234,13 @@
     <t>No. Orden</t>
   </si>
   <si>
+    <t>Tipo de orden</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tipo de vino </t>
   </si>
   <si>
     <t>Tipo de botella</t>
-  </si>
-  <si>
-    <t>Tipo de orden</t>
   </si>
   <si>
     <t>Cantidad de botellas</t>
@@ -272,17 +266,16 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -473,6 +466,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -499,24 +493,25 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -577,17 +572,13 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -595,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -626,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -634,36 +625,22 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>25</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981A18DD-35D3-406F-B05E-CB2A5EA7AB04}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,13 +657,13 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
@@ -697,7 +674,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -714,7 +691,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -731,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -748,7 +725,7 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -765,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -782,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -799,7 +776,7 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -816,7 +793,7 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -833,7 +810,7 @@
         <v>2</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -850,7 +827,7 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -867,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -884,7 +861,7 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -901,7 +878,7 @@
         <v>2</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -1310,12 +1287,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,7 +1307,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
@@ -1448,7 +1425,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>